<commit_message>
Thêm cột Hc category và Phút tăng ca ăn tối bảng công chốt
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3292CCE5-4A5E-4C1A-9F0F-0F0449AD657E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1DF97F-F396-4A9D-A96B-DABF4BE7DCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Nhà máy</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Phút tăng ca 150%</t>
   </si>
   <si>
-    <t>Phút tăng đêm</t>
-  </si>
-  <si>
     <t>Phút nghỉ không lương</t>
   </si>
   <si>
@@ -86,6 +83,15 @@
   </si>
   <si>
     <t>BẢNG CHẤM CÔNG CHI TIẾT CHỐT</t>
+  </si>
+  <si>
+    <t>HC Category</t>
+  </si>
+  <si>
+    <t>Phút tăng ca ăn tối</t>
+  </si>
+  <si>
+    <t>Phút tăng ca đêm</t>
   </si>
 </sst>
 </file>
@@ -191,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -227,6 +233,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +541,7 @@
   <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,15 +561,17 @@
     <col min="13" max="13" width="17" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" customWidth="1"/>
     <col min="19" max="20" width="16" customWidth="1"/>
     <col min="21" max="21" width="12" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -679,7 +690,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>5</v>
@@ -712,19 +723,25 @@
         <v>14</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>19</v>
+      <c r="V4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thay đổi format mục 7 cho gọn hơn, in ra theo mẫu như mục 12
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DF1DC8-4782-4D5D-9DD0-37BD318FE77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81F999B-C165-47E9-B226-F5A7B5624CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,24 +140,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -194,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -214,22 +196,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ4"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,7 +516,7 @@
     <col min="2" max="2" width="11" customWidth="1"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
@@ -563,29 +535,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
       <c r="AM1" s="3"/>
       <c r="AN1" s="3"/>
       <c r="AO1" s="3"/>
@@ -593,151 +565,105 @@
       <c r="AQ1" s="4"/>
     </row>
     <row r="2" spans="1:43" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
       <c r="AP2" s="6"/>
       <c r="AQ2" s="6"/>
     </row>
-    <row r="3" spans="1:43" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="12"/>
-      <c r="AB3" s="12"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="12"/>
-      <c r="AE3" s="12"/>
-      <c r="AF3" s="12"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="12"/>
-      <c r="AI3" s="12"/>
-      <c r="AJ3" s="12"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="12"/>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="8"/>
-      <c r="AQ3" s="8"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:U1"/>
     <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:AL3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Đồng bộ các file mẫu bảng chấm công và làm thêm giờ phần 7 và 12
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81F999B-C165-47E9-B226-F5A7B5624CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F2F1AE-BB31-4796-9099-6B3BAF754BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>